<commit_message>
Bisschen an Aufgabe 2 gemacht
</commit_message>
<xml_diff>
--- a/Doc/Messdaten.xlsx
+++ b/Doc/Messdaten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris Klobke\Documents\GitHub\MesstechnikBericht1\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A1BEAB-D6C6-4F49-AB2C-08AD56D64AE6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022B696D-E5B8-4205-A02A-30C2509AEF54}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="41">
   <si>
     <t>V1: Temperaturmessung mit PT100 &amp; Thermoelement</t>
   </si>
@@ -172,6 +172,12 @@
   <si>
     <t>Lin</t>
   </si>
+  <si>
+    <t>Thermo Reg</t>
+  </si>
+  <si>
+    <t>Thermo Delt</t>
+  </si>
 </sst>
 </file>
 
@@ -179,8 +185,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0000%"/>
-    <numFmt numFmtId="169" formatCode="0.000000%"/>
+    <numFmt numFmtId="165" formatCode="0.0000%"/>
+    <numFmt numFmtId="166" formatCode="0.000000%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -226,12 +232,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -286,7 +298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -331,8 +343,17 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -1484,6 +1505,521 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Thermospannung</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$E$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Thermo/mV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$7:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>21.1191</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61.556399999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120.833</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>180.624</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>241.03</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>301.233</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$E$7:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.84199999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9859999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3780000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.7560000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-89C2-4901-A25E-AE3514EC9AB9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1570234063"/>
+        <c:axId val="1804087663"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1570234063"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>T/°C</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1804087663"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1804087663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>U/mV</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1570234063"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1564,6 +2100,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2081,6 +2657,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2665,6 +3757,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>138111</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE0FBA79-0705-427A-B3D7-4B1016322C3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2936,10 +4064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2947,15 +4075,16 @@
     <col min="1" max="1" width="8.42578125" style="14" customWidth="1"/>
     <col min="2" max="8" width="15.7109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="2"/>
+    <col min="10" max="10" width="15.140625" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2975,7 +4104,7 @@
         <v>43783</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="8"/>
       <c r="C3" s="5"/>
@@ -2983,18 +4112,19 @@
       <c r="E3" s="3"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
+      <c r="H4" s="19"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -3022,8 +4152,14 @@
       <c r="I6" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="J6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
@@ -3055,8 +4191,16 @@
         <f>(D7-F7)/(213.621-109.133)</f>
         <v>-6.2833646925962664E-3</v>
       </c>
+      <c r="J7" s="17">
+        <f>0.0405*B7+0.0344</f>
+        <v>0.88972355000000003</v>
+      </c>
+      <c r="K7" s="17">
+        <f>E7-J7</f>
+        <v>-4.7723550000000059E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
@@ -3088,41 +4232,57 @@
         <f t="shared" ref="I8:I12" si="3">(D8-F8)/(213.621-109.133)</f>
         <v>-1.1190605619779237E-4</v>
       </c>
+      <c r="J8" s="17">
+        <f t="shared" ref="J8:J12" si="4">0.0405*B8+0.0344</f>
+        <v>2.5274342000000001</v>
+      </c>
+      <c r="K8" s="17">
+        <f t="shared" ref="K8:K12" si="5">E8-J8</f>
+        <v>-7.4342000000000574E-3</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
+    <row r="9" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20">
         <v>120</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="21">
         <v>120.833</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="21">
         <v>146.39699999999999</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="21">
         <v>147.49299999999999</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="21">
         <v>4.9859999999999998</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="21">
         <f t="shared" si="0"/>
         <v>146.99279229999999</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="22">
         <f>100*(1+3.90802*(10^-3)*B9-5.80195*(10^-7)*(B9^2))</f>
         <v>146.37465774846714</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="23">
         <f t="shared" si="2"/>
         <v>0.50020770000000425</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="24">
         <f t="shared" si="3"/>
         <v>4.7872262843580522E-3</v>
       </c>
+      <c r="J9" s="23">
+        <f t="shared" si="4"/>
+        <v>4.9281364999999999</v>
+      </c>
+      <c r="K9" s="23">
+        <f t="shared" si="5"/>
+        <v>5.7863499999999846E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>14</v>
       </c>
@@ -3154,8 +4314,16 @@
         <f t="shared" si="3"/>
         <v>6.8446673302198554E-3</v>
       </c>
+      <c r="J10" s="17">
+        <f t="shared" si="4"/>
+        <v>7.349672</v>
+      </c>
+      <c r="K10" s="17">
+        <f t="shared" si="5"/>
+        <v>2.8328000000000131E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>15</v>
       </c>
@@ -3187,8 +4355,16 @@
         <f t="shared" si="3"/>
         <v>1.0595187964169972E-3</v>
       </c>
+      <c r="J11" s="17">
+        <f t="shared" si="4"/>
+        <v>9.7961150000000004</v>
+      </c>
+      <c r="K11" s="17">
+        <f t="shared" si="5"/>
+        <v>-4.0115000000000123E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>16</v>
       </c>
@@ -3220,13 +4396,21 @@
         <f t="shared" si="3"/>
         <v>-6.4986630043640282E-3</v>
       </c>
+      <c r="J12" s="17">
+        <f t="shared" si="4"/>
+        <v>12.2343365</v>
+      </c>
+      <c r="K12" s="17">
+        <f t="shared" si="5"/>
+        <v>-3.4336500000000214E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="2" t="s">
         <v>18</v>
@@ -3238,7 +4422,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Fazit zu Aufgabe 2 und Aufgabe 4 fertich
</commit_message>
<xml_diff>
--- a/Doc/Messdaten.xlsx
+++ b/Doc/Messdaten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris Klobke\Documents\GitHub\MesstechnikBericht1\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022B696D-E5B8-4205-A02A-30C2509AEF54}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04BEAD9-D001-4229-AF8C-F37E145C22EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>V1: Temperaturmessung mit PT100 &amp; Thermoelement</t>
   </si>
@@ -183,10 +183,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
     <numFmt numFmtId="166" formatCode="0.000000%"/>
+    <numFmt numFmtId="168" formatCode="0.000%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -298,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -354,6 +355,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -1629,38 +1631,8 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -3764,16 +3736,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>138111</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>357186</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>552449</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4064,10 +4036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4079,12 +4051,12 @@
     <col min="11" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -4104,7 +4076,7 @@
         <v>43783</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="8"/>
       <c r="C3" s="5"/>
@@ -4112,19 +4084,19 @@
       <c r="E3" s="3"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="19"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -4159,7 +4131,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
@@ -4199,8 +4171,12 @@
         <f>E7-J7</f>
         <v>-4.7723550000000059E-2</v>
       </c>
+      <c r="L7" s="25">
+        <f>(E7-J7)/($E$12-$E$7)</f>
+        <v>-4.2017564712097258E-3</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
@@ -4240,8 +4216,12 @@
         <f t="shared" ref="K8:K12" si="5">E8-J8</f>
         <v>-7.4342000000000574E-3</v>
       </c>
+      <c r="L8" s="25">
+        <f t="shared" ref="L8:L12" si="6">(E8-J8)/($E$12-$E$7)</f>
+        <v>-6.5453424898750294E-4</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>120</v>
       </c>
@@ -4281,8 +4261,12 @@
         <f t="shared" si="5"/>
         <v>5.7863499999999846E-2</v>
       </c>
+      <c r="L9" s="25">
+        <f t="shared" si="6"/>
+        <v>5.0945148793801595E-3</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>14</v>
       </c>
@@ -4322,8 +4306,12 @@
         <f t="shared" si="5"/>
         <v>2.8328000000000131E-2</v>
       </c>
+      <c r="L10" s="25">
+        <f t="shared" si="6"/>
+        <v>2.4941010741327818E-3</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>15</v>
       </c>
@@ -4363,8 +4351,12 @@
         <f t="shared" si="5"/>
         <v>-4.0115000000000123E-2</v>
       </c>
+      <c r="L11" s="25">
+        <f t="shared" si="6"/>
+        <v>-3.5318718084169859E-3</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>16</v>
       </c>
@@ -4404,13 +4396,17 @@
         <f t="shared" si="5"/>
         <v>-3.4336500000000214E-2</v>
       </c>
+      <c r="L12" s="25">
+        <f t="shared" si="6"/>
+        <v>-3.0231114632858088E-3</v>
+      </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="2" t="s">
         <v>18</v>
@@ -4422,7 +4418,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>21</v>
       </c>

</xml_diff>